<commit_message>
adding week of experiments and analyses
</commit_message>
<xml_diff>
--- a/experiments/20201023_exp8_controls_gfp_atp/20201023_exp8_plan.xlsx
+++ b/experiments/20201023_exp8_controls_gfp_atp/20201023_exp8_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ankitaroychoudhury/Documents/MURRAY/ug_murray/experiments/20201023_exp8_controls_gfp_atp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B303B25-3DD9-2D4C-A7ED-1F6E9B2380F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0123CA8-1015-C04A-A9C9-0BEC99BB4AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4220" yWindow="460" windowWidth="24240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1419,8 +1419,8 @@
   </sheetPr>
   <dimension ref="A1:AQ51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1873,7 +1873,7 @@
         <v>7.88</v>
       </c>
       <c r="I12" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>114</v>

</xml_diff>